<commit_message>
EPBDS-7960 Add a new test
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7960_min_with_StringOperators.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7960_min_with_StringOperators.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Step</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Test getMin1 testGetMin1</t>
+  </si>
+  <si>
+    <t>Test getMin3 testGetMin3</t>
+  </si>
+  <si>
+    <t>Spreadsheet Object getMin3(double a, String b)</t>
+  </si>
+  <si>
+    <t>In StringOperators typeToString has a bigger distance than stringToType. So it's assumed that here min(double, double) will be used (instead of min(String, String))</t>
   </si>
 </sst>
 </file>
@@ -527,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:E29"/>
+  <dimension ref="C2:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -541,7 +550,7 @@
     <col min="4" max="4" width="25.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="24.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="25.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="38.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="12.85546875" style="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12.85546875" style="1" customWidth="1" collapsed="1"/>
@@ -713,10 +722,96 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="C36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C41" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C45" s="1">
+        <v>12</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E45" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C46" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D46" s="1">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="E46" s="1">
+        <v>-1.1000000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>